<commit_message>
doc: add instructions for input
</commit_message>
<xml_diff>
--- a/mobipy/domain/accountancy/lodger.xlsx
+++ b/mobipy/domain/accountancy/lodger.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="14480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="identity" sheetId="1" r:id="rId1"/>
@@ -27,70 +27,70 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
+    <t>rentable</t>
+  </si>
+  <si>
+    <t>lodger</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mobile_phone</t>
+  </si>
+  <si>
+    <t>home_phone</t>
+  </si>
+  <si>
+    <t>entry_date</t>
+  </si>
+  <si>
+    <t>exit_date</t>
+  </si>
+  <si>
+    <t>expenditure</t>
+  </si>
+  <si>
+    <t>rent</t>
+  </si>
+  <si>
+    <t>Jean</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Dupont</t>
+  </si>
+  <si>
+    <t>DesMerveilles</t>
+  </si>
+  <si>
+    <t>Albert</t>
+  </si>
+  <si>
+    <t>Harper</t>
+  </si>
+  <si>
+    <t>blomet</t>
+  </si>
+  <si>
+    <t>ivry</t>
+  </si>
+  <si>
     <t>_id</t>
-  </si>
-  <si>
-    <t>rentable</t>
-  </si>
-  <si>
-    <t>lodger</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>mobile_phone</t>
-  </si>
-  <si>
-    <t>home_phone</t>
-  </si>
-  <si>
-    <t>entry_date</t>
-  </si>
-  <si>
-    <t>exit_date</t>
-  </si>
-  <si>
-    <t>expenditure</t>
-  </si>
-  <si>
-    <t>rent</t>
-  </si>
-  <si>
-    <t>Jean</t>
-  </si>
-  <si>
-    <t>Alice</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
-    <t>Dupont</t>
-  </si>
-  <si>
-    <t>DesMerveilles</t>
-  </si>
-  <si>
-    <t>Albert</t>
-  </si>
-  <si>
-    <t>Harper</t>
-  </si>
-  <si>
-    <t>blomet</t>
-  </si>
-  <si>
-    <t>ivry</t>
   </si>
 </sst>
 </file>
@@ -409,12 +409,11 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -423,22 +422,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -446,10 +445,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -457,10 +456,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -468,10 +467,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -479,10 +478,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -495,12 +494,11 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
@@ -508,25 +506,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -534,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -557,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -580,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -600,7 +598,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -620,7 +618,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>3</v>

</xml_diff>